<commit_message>
filled excel dummy data
</commit_message>
<xml_diff>
--- a/Npoi.Mapper/test/Book1.xlsx
+++ b/Npoi.Mapper/test/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="0" windowWidth="24120" windowHeight="12795"/>
+    <workbookView xWindow="12090" yWindow="0" windowWidth="24120" windowHeight="12795" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RESources" sheetId="2" r:id="rId1"/>
@@ -25,13 +25,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
-    <t>frank_zh_wu@manulife-sinochem.com</t>
-  </si>
-  <si>
     <t>Frank Wu</t>
-  </si>
-  <si>
-    <t>donny_d_tian@manulife-sinochem.com</t>
   </si>
   <si>
     <t>Donny Tian</t>
@@ -185,6 +179,14 @@
   </si>
   <si>
     <t>Done by Excel and provide upload functionality.</t>
+  </si>
+  <si>
+    <t>donny@example.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>frank@example.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -612,7 +614,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -622,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
@@ -635,26 +637,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -683,170 +685,170 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -873,24 +875,24 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3">
         <v>42430</v>
@@ -901,10 +903,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3">
         <v>42430</v>
@@ -915,10 +917,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3">
         <v>42401</v>
@@ -938,9 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -951,10 +951,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C1" s="3">
         <v>42461</v>
@@ -974,10 +974,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -1017,10 +1017,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -1070,7 +1070,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1085,22 +1085,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="7" customFormat="1">
       <c r="A1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.5">
@@ -1108,19 +1108,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
fix #4 v2.1 support Nullable property mapping mark the method to use builtin format as obsolete
</commit_message>
<xml_diff>
--- a/Npoi.Mapper/test/Book1.xlsx
+++ b/Npoi.Mapper/test/Book1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\src\github\Npoi.Mapper\Npoi.Mapper\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="0" windowWidth="24120" windowHeight="12795" activeTab="3"/>
+    <workbookView xWindow="16740" yWindow="0" windowWidth="24120" windowHeight="12795" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="RESources" sheetId="2" r:id="rId1"/>
@@ -12,6 +17,8 @@
     <sheet name="Allocations" sheetId="3" r:id="rId3"/>
     <sheet name="QuickAllocate" sheetId="5" r:id="rId4"/>
     <sheet name="Backlogs" sheetId="4" r:id="rId5"/>
+    <sheet name="TestClass" sheetId="6" r:id="rId6"/>
+    <sheet name="NullableClass" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -23,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
   <si>
     <t>Frank Wu</t>
   </si>
@@ -186,17 +193,69 @@
   </si>
   <si>
     <t>frank@example.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DateTime</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Double</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017/01/01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2345</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal case</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>this row need to be converted</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>this row need to be parsed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>123.45%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NullableDateTime</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid value should result a null property</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>01^01^2017</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>01^01^2017</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-409]mmmm\-yy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,7 +339,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -306,11 +365,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,7 +675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,14 +689,14 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="49.375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -643,7 +704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -651,7 +712,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,13 +738,13 @@
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.25" customWidth="1"/>
     <col min="2" max="3" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -697,7 +758,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -711,7 +772,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -725,7 +786,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -739,7 +800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -753,7 +814,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -767,7 +828,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -781,7 +842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -795,7 +856,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -809,7 +870,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -823,7 +884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -837,7 +898,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -865,7 +926,7 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="33.125" customWidth="1"/>
@@ -873,7 +934,7 @@
     <col min="4" max="4" width="36.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -887,7 +948,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -901,7 +962,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -915,7 +976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -940,16 +1001,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="24.75" customWidth="1"/>
     <col min="3" max="7" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -972,7 +1033,7 @@
         <v>42583</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -995,7 +1056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -1015,7 +1076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -1073,7 +1134,7 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.25" customWidth="1"/>
     <col min="2" max="2" width="47.625" bestFit="1" customWidth="1"/>
@@ -1083,7 +1144,7 @@
     <col min="6" max="6" width="50.375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
@@ -1103,7 +1164,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.5">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1123,7 +1184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -1131,7 +1192,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -1139,7 +1200,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -1147,7 +1208,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
@@ -1155,7 +1216,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -1163,7 +1224,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
@@ -1171,7 +1232,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
@@ -1179,7 +1240,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="9"/>
@@ -1187,7 +1248,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="9"/>
@@ -1195,7 +1256,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
@@ -1203,7 +1264,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -1211,7 +1272,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
@@ -1219,7 +1280,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
@@ -1227,7 +1288,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
@@ -1235,7 +1296,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
@@ -1243,7 +1304,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
@@ -1251,7 +1312,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
@@ -1259,7 +1320,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
@@ -1267,7 +1328,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -1275,7 +1336,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
@@ -1283,7 +1344,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
@@ -1291,7 +1352,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
@@ -1299,7 +1360,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
@@ -1307,7 +1368,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
@@ -1315,7 +1376,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -1323,7 +1384,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
@@ -1331,7 +1392,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="8"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
@@ -1343,4 +1404,114 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="11">
+        <v>42736</v>
+      </c>
+      <c r="C2">
+        <v>0.56779999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix #8 No error reported for nullable value type columns during import added IgnoreErrorsFor to suppress errors on specific column
</commit_message>
<xml_diff>
--- a/Npoi.Mapper/test/Book1.xlsx
+++ b/Npoi.Mapper/test/Book1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Frank Wu</t>
   </si>
@@ -245,6 +245,26 @@
   </si>
   <si>
     <t>01^01^2017</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NormalString</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1473,40 +1493,56 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>42736</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add SkipRows to skip certain number of lines from beginning By demo  var importer = new Mapper(stream);  var items = importer.SkipRows(1).Take<dynamic>("Skip").ToList();
</commit_message>
<xml_diff>
--- a/Npoi.Mapper/test/Book1.xlsx
+++ b/Npoi.Mapper/test/Book1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\src\github\Npoi.Mapper\Npoi.Mapper\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Desktop\abp\Npoi.Mapper\Npoi.Mapper\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BBEB42-CFFE-42E5-BD61-6C36C19CFF6B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="0" windowWidth="24120" windowHeight="12795" activeTab="6"/>
+    <workbookView xWindow="16740" yWindow="0" windowWidth="24120" windowHeight="12795" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RESources" sheetId="2" r:id="rId1"/>
@@ -19,6 +20,7 @@
     <sheet name="Backlogs" sheetId="4" r:id="rId5"/>
     <sheet name="TestClass" sheetId="6" r:id="rId6"/>
     <sheet name="NullableClass" sheetId="7" r:id="rId7"/>
+    <sheet name="Skip" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="79">
   <si>
     <t>Frank Wu</t>
   </si>
@@ -249,6 +251,47 @@
   </si>
   <si>
     <t>NormalString</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">币种          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">对方户名       </t>
+  </si>
+  <si>
+    <t>20180914 10:45:30</t>
+  </si>
+  <si>
+    <t>人民币元</t>
+  </si>
+  <si>
+    <t>江苏省常熟环通实业有限公司</t>
+  </si>
+  <si>
+    <t>20180914 10:45:31</t>
+  </si>
+  <si>
+    <t>合肥春盎然商贸有限公司</t>
+  </si>
+  <si>
+    <t>交易记录</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -271,11 +314,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="[$-409]mmmm\-yy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,6 +353,11 @@
       <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -359,7 +407,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -387,11 +435,17 @@
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -702,7 +756,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -743,15 +797,15 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -939,7 +993,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1018,7 +1072,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1147,7 +1201,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1427,7 +1481,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1492,10 +1546,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1550,4 +1604,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6ED8DA8-284E-4324-9BA5-54EC4E73B4FE}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="15">
+        <v>858.37</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>23935542.370000001</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="15">
+        <v>79.47</v>
+      </c>
+      <c r="C4" s="15">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>23935462.899999999</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>